<commit_message>
Update Specification & Plannification
</commit_message>
<xml_diff>
--- a/Documentation/Planification_V1.xlsx
+++ b/Documentation/Planification_V1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/371c2caacf93074d/Documents/HEIG/TB Driver Brushless/TB-Driver-Brushless/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CB7147DC-5DFD-4F3C-85F9-1BD4040EC95A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="93" documentId="8_{CB7147DC-5DFD-4F3C-85F9-1BD4040EC95A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{F103D6D7-A7BD-4156-83DC-A0C8225237DE}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="672" windowWidth="17280" windowHeight="8976" xr2:uid="{E4DCEC7E-A84B-4A69-AC68-472FA9C158BB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E4DCEC7E-A84B-4A69-AC68-472FA9C158BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>N°</t>
   </si>
@@ -90,9 +90,6 @@
     <t>Programmation</t>
   </si>
   <si>
-    <t>Tests</t>
-  </si>
-  <si>
     <t>Écriture du rapport</t>
   </si>
   <si>
@@ -117,9 +114,6 @@
     <t>Rédaction de documents livrables</t>
   </si>
   <si>
-    <t>Gestion du projet (~10%)</t>
-  </si>
-  <si>
     <t>T90</t>
   </si>
   <si>
@@ -129,9 +123,6 @@
     <t>Mesures des performances</t>
   </si>
   <si>
-    <t>T100</t>
-  </si>
-  <si>
     <t>Dessin du schéma électrique</t>
   </si>
   <si>
@@ -153,9 +144,6 @@
     <t>Gestion d'un codeur absolu analogique</t>
   </si>
   <si>
-    <t>Communication I2C</t>
-  </si>
-  <si>
     <t>Communication CAN</t>
   </si>
   <si>
@@ -183,9 +171,6 @@
     <t>T80.20</t>
   </si>
   <si>
-    <t>T90.10</t>
-  </si>
-  <si>
     <t>T50.10</t>
   </si>
   <si>
@@ -211,14 +196,58 @@
   </si>
   <si>
     <t>Imprévus (~10% = 42H)</t>
+  </si>
+  <si>
+    <t>Communication I2C / SPI</t>
+  </si>
+  <si>
+    <t>T50.90</t>
+  </si>
+  <si>
+    <t>Communication UART</t>
+  </si>
+  <si>
+    <t>T50.100</t>
+  </si>
+  <si>
+    <t>Gestion du pont triphasé</t>
+  </si>
+  <si>
+    <t>T70.10</t>
+  </si>
+  <si>
+    <t>T70.20</t>
+  </si>
+  <si>
+    <t>Séances ébdomadaires avec prof. Répondant (préparation)</t>
+  </si>
+  <si>
+    <t>Gestion du projet</t>
+  </si>
+  <si>
+    <t>Schéma de puissance</t>
+  </si>
+  <si>
+    <t>Schéma de commande</t>
+  </si>
+  <si>
+    <t>Schéma d'alimentations</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -246,12 +275,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -568,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09FBCC03-12B2-4877-A171-7A10D6B76BA3}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -585,22 +618,22 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
+      <c r="C1" s="2"/>
       <c r="D1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1"/>
+      <c r="C2" s="4"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -637,261 +670,338 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D6">
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C7" s="1"/>
-      <c r="D7">
-        <v>40</v>
-      </c>
+      <c r="A7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="4"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D10">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B11" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8">
+      <c r="C11" s="4"/>
+      <c r="D11">
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="1" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C12" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="1"/>
-      <c r="D13">
-        <v>120</v>
-      </c>
+      <c r="C13" s="4"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2" t="s">
-        <v>33</v>
+        <v>40</v>
+      </c>
+      <c r="C14" t="s">
+        <v>14</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C15" t="s">
-        <v>34</v>
+        <v>15</v>
+      </c>
+      <c r="D15">
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="C16" t="s">
-        <v>35</v>
+        <v>16</v>
+      </c>
+      <c r="D16">
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>53</v>
-      </c>
-      <c r="C17" t="s">
-        <v>36</v>
-      </c>
+      <c r="A17" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="4"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>54</v>
-      </c>
-      <c r="C18" t="s">
-        <v>37</v>
+        <v>45</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D18">
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>55</v>
-      </c>
-      <c r="C19" t="s">
-        <v>38</v>
+        <v>46</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19">
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>31</v>
+      </c>
+      <c r="D20">
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C21" t="s">
-        <v>40</v>
+        <v>32</v>
+      </c>
+      <c r="D21">
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" s="1"/>
+        <v>49</v>
+      </c>
+      <c r="C22" t="s">
+        <v>33</v>
+      </c>
       <c r="D22">
         <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C23" s="1"/>
+        <v>50</v>
+      </c>
+      <c r="C23" t="s">
+        <v>34</v>
+      </c>
       <c r="D23">
         <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="1"/>
+        <v>51</v>
+      </c>
+      <c r="C24" t="s">
+        <v>35</v>
+      </c>
       <c r="D24">
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C25" t="s">
-        <v>19</v>
+        <v>54</v>
+      </c>
+      <c r="D25">
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="C26" t="s">
-        <v>20</v>
+        <v>36</v>
+      </c>
+      <c r="D26">
+        <v>25</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="C28" s="4"/>
+      <c r="D28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="4"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31" t="s">
+        <v>18</v>
+      </c>
+      <c r="D31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" t="s">
+        <v>19</v>
+      </c>
+      <c r="D32">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C33" s="4"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>43</v>
+      </c>
+      <c r="C34" t="s">
         <v>27</v>
       </c>
-      <c r="C27" s="1"/>
-      <c r="D27">
+      <c r="D34">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>44</v>
+      </c>
+      <c r="C35" t="s">
+        <v>61</v>
+      </c>
+      <c r="D35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C36" s="4"/>
+      <c r="D36">
         <v>42</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>49</v>
-      </c>
-      <c r="C28" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>31</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" s="1"/>
-      <c r="D29">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="D31">
-        <f>SUM(D2:D29)</f>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D38">
+        <f>SUM(D2:D36)</f>
         <v>420</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B29:C29"/>
+  <mergeCells count="10">
+    <mergeCell ref="B17:C17"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B11:C11"/>
     <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B36:C36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>